<commit_message>
POI：bug 58339: patch from Patrick Zimmermann to allow OFFSET() to accept missing optional width or height parameters
</commit_message>
<xml_diff>
--- a/testcases/test-data/spreadsheet/FormulaEvalTestData_Copy.xlsx
+++ b/testcases/test-data/spreadsheet/FormulaEvalTestData_Copy.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="-210" windowWidth="12120" windowHeight="9120" tabRatio="452"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" tabRatio="452"/>
   </bookViews>
   <sheets>
     <sheet name="EverythingTests" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="StatsLibTests" sheetId="3" r:id="rId3"/>
     <sheet name="misc" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -22,7 +27,7 @@
     <author>Amol</author>
   </authors>
   <commentList>
-    <comment ref="B420" authorId="0">
+    <comment ref="B420" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3725,12 +3730,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="180" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="181" formatCode="0.00000000000"/>
-    <numFmt numFmtId="182" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="184" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="189" formatCode="0.0000"/>
-    <numFmt numFmtId="192" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="167" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -3982,9 +3987,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -4007,7 +4012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyProtection="1">
@@ -4049,7 +4054,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="184" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
@@ -4067,14 +4072,14 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="189" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="189" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="192" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
@@ -4136,6 +4141,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4183,7 +4191,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4218,7 +4226,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4430,11 +4438,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:AL1504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <pane xSplit="16230" ySplit="3840" topLeftCell="AQ58" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <pane xSplit="16230" ySplit="3840" topLeftCell="AQ1000" activePane="bottomLeft"/>
       <selection activeCell="A6" sqref="A6:A21"/>
       <selection pane="topRight" activeCell="AQ16" sqref="AQ16"/>
-      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
+      <selection pane="bottomLeft" activeCell="L1008" sqref="L1008"/>
       <selection pane="bottomRight" activeCell="AI1443" sqref="AI1443"/>
     </sheetView>
   </sheetViews>
@@ -14714,8 +14722,36 @@
         <f ca="1">OFFSET(F7, E7:I7, E7:I7)</f>
         <v>1.0009999999999999</v>
       </c>
-    </row>
-    <row r="1009" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H1008" s="2">
+        <f ca="1">SUM(OFFSET(K7:L8, 0,0,1,1))</f>
+        <v>1</v>
+      </c>
+      <c r="I1008" s="2">
+        <f ca="1">SUM(OFFSET(K7:L8, 0,0,1,))</f>
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="J1008" s="2">
+        <f ca="1">SUM(OFFSET(K7:L8, 0,0,,1))</f>
+        <v>3</v>
+      </c>
+      <c r="K1008" s="2">
+        <f ca="1">SUM(OFFSET(K7:L8, 0,0,1))</f>
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="L1008" s="2">
+        <f ca="1">SUM(OFFSET(K7:L8, 0,0))</f>
+        <v>7.0008999999999997</v>
+      </c>
+      <c r="M1008" s="2">
+        <f ca="1">SUM(OFFSET(K7:L8, 0,0,,))</f>
+        <v>7.0008999999999997</v>
+      </c>
+      <c r="N1008" s="2">
+        <f ca="1">SUM(OFFSET(K7:L8, 0,0,))</f>
+        <v>7.0008999999999997</v>
+      </c>
+    </row>
+    <row r="1009" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C1009" s="1" t="s">
         <v>428</v>
       </c>
@@ -14731,8 +14767,29 @@
       <c r="G1009" s="2">
         <v>1.0009999999999999</v>
       </c>
-    </row>
-    <row r="1012" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H1009" s="2">
+        <v>1</v>
+      </c>
+      <c r="I1009" s="2">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="J1009" s="2">
+        <v>3</v>
+      </c>
+      <c r="K1009" s="2">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="L1009" s="2">
+        <v>7.0008999999999997</v>
+      </c>
+      <c r="M1009" s="2">
+        <v>7.0008999999999997</v>
+      </c>
+      <c r="N1009" s="2">
+        <v>7.0008999999999997</v>
+      </c>
+    </row>
+    <row r="1012" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B1012" s="1" t="s">
         <v>429</v>
       </c>
@@ -14743,7 +14800,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="1013" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1013" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C1013" s="1" t="s">
         <v>431</v>
       </c>
@@ -14751,7 +14808,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="1016" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1016" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B1016" s="1" t="s">
         <v>432</v>
       </c>
@@ -14762,7 +14819,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="1017" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1017" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C1017" s="1" t="s">
         <v>434</v>
       </c>
@@ -14770,7 +14827,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="1020" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1020" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B1020" s="1" t="s">
         <v>435</v>
       </c>
@@ -14810,7 +14867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1021" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1021" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C1021" s="1" t="s">
         <v>437</v>
       </c>
@@ -14839,7 +14896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1024" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1024" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B1024" s="1" t="s">
         <v>438</v>
       </c>
@@ -19137,14 +19194,13 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="6">
+    <mergeCell ref="B94:C94"/>
     <mergeCell ref="T6:Z6"/>
     <mergeCell ref="B2:M4"/>
     <mergeCell ref="A6:A21"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="K6:O6"/>
-    <mergeCell ref="B94:C94"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>

</xml_diff>